<commit_message>
profit calculations in 3-hour intervals based on hashrate, price, and local energy prices
</commit_message>
<xml_diff>
--- a/data_and_scripts/costsNEW.xlsx
+++ b/data_and_scripts/costsNEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riius/Desktop/Bitcoin gametheory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riius/bitcoin-mining-gametheory/data_and_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63864370-4AC8-FC45-B9FE-28A8BEF4D765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADDFD10-A267-C740-A70E-225CFE9A3D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="280" windowWidth="38400" windowHeight="21600" xr2:uid="{4254AAF4-7B1B-7A49-BC49-03C28463EAF9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4254AAF4-7B1B-7A49-BC49-03C28463EAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -831,8 +831,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>